<commit_message>
Achieve first working version of Royalty_Calculator - physical only
Resolve keyErrors in code, fix net-rate calculation, fix penny-rate handling, add item to TODO, create first royalty-run spreadsheet
</commit_message>
<xml_diff>
--- a/Physical_Sales.xlsx
+++ b/Physical_Sales.xlsx
@@ -1877,9 +1877,6 @@
     <t>sale-month</t>
   </si>
   <si>
-    <t>upc-ean</t>
-  </si>
-  <si>
     <t>Bleep</t>
   </si>
   <si>
@@ -2429,6 +2426,9 @@
   </si>
   <si>
     <t>Something Old, Something New, Something Borrowed Blues</t>
+  </si>
+  <si>
+    <t>upc</t>
   </si>
 </sst>
 </file>
@@ -2873,7 +2873,7 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2900,7 +2900,7 @@
         <v>485</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -2909,18 +2909,18 @@
         <v>482</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>486</v>
+        <v>668</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>480</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -2929,19 +2929,19 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G2" s="7">
         <v>652905010112</v>
       </c>
       <c r="H2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I2">
         <v>112</v>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -2958,19 +2958,19 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G3" s="7">
         <v>652905010129</v>
       </c>
       <c r="H3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I3">
         <v>39</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4">
         <v>2022</v>
@@ -2987,19 +2987,19 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G4" s="8">
         <v>652905010228</v>
       </c>
       <c r="H4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B5">
         <v>2022</v>
@@ -3016,19 +3016,19 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G5" s="8">
         <v>652905010327</v>
       </c>
       <c r="H5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I5">
         <v>13</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B6">
         <v>2022</v>
@@ -3045,19 +3045,19 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G6" s="8">
         <v>652905010426</v>
       </c>
       <c r="H6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I6">
         <v>20</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B7">
         <v>2022</v>
@@ -3074,19 +3074,19 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G7" s="8">
         <v>652905010518</v>
       </c>
       <c r="H7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I7">
         <v>128</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B8">
         <v>2022</v>
@@ -3103,19 +3103,19 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G8" s="8">
         <v>652905010525</v>
       </c>
       <c r="H8" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I8">
         <v>39</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B9">
         <v>2022</v>
@@ -3132,19 +3132,19 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G9" s="8">
         <v>652905010624</v>
       </c>
       <c r="H9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I9">
         <v>7</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B10">
         <v>2022</v>
@@ -3161,19 +3161,19 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G10" s="8">
         <v>652905010723</v>
       </c>
       <c r="H10" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I10">
         <v>14</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B11">
         <v>2022</v>
@@ -3190,19 +3190,19 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G11" s="8">
         <v>652905010822</v>
       </c>
       <c r="H11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B12">
         <v>2022</v>
@@ -3219,19 +3219,19 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G12" s="8">
         <v>652905010914</v>
       </c>
       <c r="H12" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I12">
         <v>225</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B13">
         <v>2022</v>
@@ -3248,19 +3248,19 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G13" s="8">
         <v>652905010921</v>
       </c>
       <c r="H13" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I13">
         <v>178</v>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B14">
         <v>2022</v>
@@ -3277,19 +3277,19 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G14" s="8">
         <v>652905011126</v>
       </c>
       <c r="H14" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I14">
         <v>33</v>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B15">
         <v>2022</v>
@@ -3306,19 +3306,19 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G15" s="8">
         <v>652905011225</v>
       </c>
       <c r="H15" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I15">
         <v>7</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B16">
         <v>2022</v>
@@ -3335,19 +3335,19 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G16" s="8">
         <v>652905011324</v>
       </c>
       <c r="H16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I16">
         <v>21</v>
@@ -3355,7 +3355,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B17">
         <v>2022</v>
@@ -3364,19 +3364,19 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G17" s="8">
         <v>652905011423</v>
       </c>
       <c r="H17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I17">
         <v>61</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B18">
         <v>2022</v>
@@ -3393,19 +3393,19 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G18" s="8">
         <v>652905011522</v>
       </c>
       <c r="H18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -3413,7 +3413,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B19">
         <v>2022</v>
@@ -3422,19 +3422,19 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G19" s="8">
         <v>652905020128</v>
       </c>
       <c r="H19" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I19">
         <v>6</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B20">
         <v>2022</v>
@@ -3451,19 +3451,19 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G20" s="8">
         <v>652905020227</v>
       </c>
       <c r="H20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B21">
         <v>2022</v>
@@ -3480,19 +3480,19 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G21" s="8">
         <v>652905020326</v>
       </c>
       <c r="H21" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I21">
         <v>9</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B22">
         <v>2022</v>
@@ -3509,19 +3509,19 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G22" s="8">
         <v>652905020425</v>
       </c>
       <c r="H22" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I22">
         <v>5</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B23">
         <v>2022</v>
@@ -3538,19 +3538,19 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G23" s="8">
         <v>652905020623</v>
       </c>
       <c r="H23" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I23">
         <v>6</v>
@@ -3558,7 +3558,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B24">
         <v>2022</v>
@@ -3567,19 +3567,19 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G24" s="8">
         <v>652905030127</v>
       </c>
       <c r="H24" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B25">
         <v>2022</v>
@@ -3596,19 +3596,19 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E25" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G25" s="8">
         <v>652905030226</v>
       </c>
       <c r="H25" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I25">
         <v>3</v>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B26">
         <v>2022</v>
@@ -3625,19 +3625,19 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E26" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G26" s="8">
         <v>652905030325</v>
       </c>
       <c r="H26" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I26">
         <v>3</v>
@@ -3645,7 +3645,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B27">
         <v>2022</v>
@@ -3654,19 +3654,19 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G27" s="8">
         <v>652905030424</v>
       </c>
       <c r="H27" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I27">
         <v>4</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B28">
         <v>2022</v>
@@ -3683,19 +3683,19 @@
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G28" s="8">
         <v>652905030523</v>
       </c>
       <c r="H28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I28">
         <v>8</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B29">
         <v>2022</v>
@@ -3712,19 +3712,19 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G29" s="8">
         <v>652905030622</v>
       </c>
       <c r="H29" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I29">
         <v>41</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B30">
         <v>2022</v>
@@ -3741,19 +3741,19 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G30" s="8">
         <v>652905040126</v>
       </c>
       <c r="H30" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I30">
         <v>2</v>
@@ -3761,7 +3761,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B31">
         <v>2022</v>
@@ -3770,19 +3770,19 @@
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G31" s="8">
         <v>652905040225</v>
       </c>
       <c r="H31" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B32">
         <v>2022</v>
@@ -3799,19 +3799,19 @@
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G32" s="8">
         <v>652905040324</v>
       </c>
       <c r="H32" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -3819,7 +3819,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B33">
         <v>2022</v>
@@ -3828,19 +3828,19 @@
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G33" s="8">
         <v>652905040423</v>
       </c>
       <c r="H33" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B34">
         <v>2022</v>
@@ -3857,19 +3857,19 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G34" s="8">
         <v>652905040522</v>
       </c>
       <c r="H34" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I34">
         <v>5</v>
@@ -3877,7 +3877,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B35">
         <v>2022</v>
@@ -3886,19 +3886,19 @@
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G35" s="10">
         <v>652905040621</v>
       </c>
       <c r="H35" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I35">
         <v>8</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B36">
         <v>2022</v>
@@ -3915,19 +3915,19 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G36" s="10">
         <v>652905040720</v>
       </c>
       <c r="H36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I36">
         <v>-12</v>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B37">
         <v>2022</v>
@@ -3944,19 +3944,19 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G37" s="10">
         <v>652905040836</v>
       </c>
       <c r="H37" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I37">
         <v>17</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B38">
         <v>2022</v>
@@ -3973,19 +3973,19 @@
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G38" s="10">
         <v>652905040928</v>
       </c>
       <c r="H38" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -3993,7 +3993,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B39">
         <v>2022</v>
@@ -4002,19 +4002,19 @@
         <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G39" s="8">
         <v>652905050125</v>
       </c>
       <c r="H39" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I39">
         <v>90</v>
@@ -4022,7 +4022,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B40">
         <v>2022</v>
@@ -4031,19 +4031,19 @@
         <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G40" s="8">
         <v>652905050224</v>
       </c>
       <c r="H40" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I40">
         <v>73</v>
@@ -4051,7 +4051,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B41">
         <v>2022</v>
@@ -4060,19 +4060,19 @@
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G41" s="8">
         <v>652905050323</v>
       </c>
       <c r="H41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I41">
         <v>5</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B42">
         <v>2022</v>
@@ -4089,19 +4089,19 @@
         <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G42" s="8">
         <v>652905050422</v>
       </c>
       <c r="H42" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I42">
         <v>18</v>
@@ -4109,7 +4109,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B43">
         <v>2022</v>
@@ -4118,19 +4118,19 @@
         <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G43" s="10">
         <v>652905050521</v>
       </c>
       <c r="H43" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I43">
         <v>12</v>
@@ -4138,7 +4138,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B44">
         <v>2022</v>
@@ -4147,19 +4147,19 @@
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G44" s="10">
         <v>652905050620</v>
       </c>
       <c r="H44" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I44">
         <v>10</v>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B45">
         <v>2022</v>
@@ -4176,19 +4176,19 @@
         <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G45" s="10">
         <v>652905050729</v>
       </c>
       <c r="H45" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I45">
         <v>55</v>
@@ -4196,7 +4196,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B46">
         <v>2022</v>
@@ -4205,19 +4205,19 @@
         <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G46" s="10">
         <v>652905050828</v>
       </c>
       <c r="H46" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I46">
         <v>179</v>
@@ -4225,7 +4225,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B47">
         <v>2022</v>
@@ -4234,19 +4234,19 @@
         <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E47" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G47" s="8">
         <v>652905060124</v>
       </c>
       <c r="H47" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B48">
         <v>2022</v>
@@ -4263,19 +4263,19 @@
         <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G48" s="8">
         <v>652905071328</v>
       </c>
       <c r="H48" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I48">
         <v>28</v>
@@ -4283,7 +4283,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B49">
         <v>2022</v>
@@ -4292,19 +4292,19 @@
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G49" s="8">
         <v>652905071717</v>
       </c>
       <c r="H49" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I49">
         <v>6</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B50">
         <v>2022</v>
@@ -4321,19 +4321,19 @@
         <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G50" s="8">
         <v>652905071724</v>
       </c>
       <c r="H50" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I50">
         <v>53</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B51">
         <v>2022</v>
@@ -4350,19 +4350,19 @@
         <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G51" s="8">
         <v>652905071823</v>
       </c>
       <c r="H51" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I51">
         <v>17</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B52">
         <v>2022</v>
@@ -4379,19 +4379,19 @@
         <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E52" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G52" s="8">
         <v>652905080122</v>
       </c>
       <c r="H52" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I52">
         <v>2</v>
@@ -4399,7 +4399,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B53">
         <v>2022</v>
@@ -4408,19 +4408,19 @@
         <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E53" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G53" s="8">
         <v>652905080221</v>
       </c>
       <c r="H53" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I53">
         <v>4</v>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B54">
         <v>2022</v>
@@ -4437,19 +4437,19 @@
         <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E54" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G54" s="8">
         <v>652905080320</v>
       </c>
       <c r="H54" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I54">
         <v>4</v>
@@ -4457,7 +4457,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B55">
         <v>2022</v>
@@ -4466,19 +4466,19 @@
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E55" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G55" s="8">
         <v>652905090121</v>
       </c>
       <c r="H55" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I55">
         <v>38</v>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B56">
         <v>2022</v>
@@ -4495,19 +4495,19 @@
         <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E56" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G56" s="8">
         <v>652905090220</v>
       </c>
       <c r="H56" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I56">
         <v>6</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B57">
         <v>2022</v>
@@ -4524,19 +4524,19 @@
         <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G57" s="8">
         <v>652905100127</v>
       </c>
       <c r="H57" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B58">
         <v>2022</v>
@@ -4553,19 +4553,19 @@
         <v>12</v>
       </c>
       <c r="D58" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G58" s="8">
         <v>652905100226</v>
       </c>
       <c r="H58" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -4573,7 +4573,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B59">
         <v>2022</v>
@@ -4582,19 +4582,19 @@
         <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G59" s="8">
         <v>652905100325</v>
       </c>
       <c r="H59" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -4602,7 +4602,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B60">
         <v>2022</v>
@@ -4611,19 +4611,19 @@
         <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G60" s="8">
         <v>652905100424</v>
       </c>
       <c r="H60" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B61">
         <v>2022</v>
@@ -4640,19 +4640,19 @@
         <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G61" s="10">
         <v>652905100523</v>
       </c>
       <c r="H61" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I61">
         <v>2</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B62">
         <v>2022</v>
@@ -4669,19 +4669,19 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E62" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G62" s="8">
         <v>652905110126</v>
       </c>
       <c r="H62" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I62">
         <v>25</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B63">
         <v>2022</v>
@@ -4698,19 +4698,19 @@
         <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G63" s="10">
         <v>652905120217</v>
       </c>
       <c r="H63" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I63">
         <v>435</v>
@@ -4718,7 +4718,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B64">
         <v>2022</v>
@@ -4727,19 +4727,19 @@
         <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G64" s="10">
         <v>652905120224</v>
       </c>
       <c r="H64" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I64">
         <v>111</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B65">
         <v>2022</v>
@@ -4756,19 +4756,19 @@
         <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G65" s="10">
         <v>652905120323</v>
       </c>
       <c r="H65" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B66">
         <v>2022</v>
@@ -4785,19 +4785,19 @@
         <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G66" s="10">
         <v>652905120415</v>
       </c>
       <c r="H66" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I66">
         <v>200</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B67">
         <v>2022</v>
@@ -4814,19 +4814,19 @@
         <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G67" s="10">
         <v>652905120422</v>
       </c>
       <c r="H67" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I67">
         <v>62</v>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B68">
         <v>2022</v>
@@ -4843,19 +4843,19 @@
         <v>12</v>
       </c>
       <c r="D68" t="s">
+        <v>511</v>
+      </c>
+      <c r="E68" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="E68" s="11" t="s">
-        <v>513</v>
-      </c>
       <c r="F68" s="12" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G68" s="10">
         <v>652905140123</v>
       </c>
       <c r="H68" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I68">
         <v>1</v>
@@ -4863,7 +4863,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B69">
         <v>2022</v>
@@ -4872,19 +4872,19 @@
         <v>12</v>
       </c>
       <c r="D69" t="s">
+        <v>511</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="E69" s="11" t="s">
-        <v>513</v>
-      </c>
       <c r="F69" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G69" s="10">
         <v>652905140222</v>
       </c>
       <c r="H69" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I69">
         <v>5</v>
@@ -4892,7 +4892,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B70">
         <v>2022</v>
@@ -4901,19 +4901,19 @@
         <v>12</v>
       </c>
       <c r="D70" t="s">
+        <v>511</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>513</v>
-      </c>
       <c r="F70" s="12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G70" s="8">
         <v>652905140420</v>
       </c>
       <c r="H70" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I70">
         <v>6</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B71">
         <v>2022</v>
@@ -4930,19 +4930,19 @@
         <v>12</v>
       </c>
       <c r="D71" t="s">
+        <v>511</v>
+      </c>
+      <c r="E71" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="E71" s="11" t="s">
-        <v>513</v>
-      </c>
       <c r="F71" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G71" s="8">
         <v>652905140628</v>
       </c>
       <c r="H71" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I71">
         <v>41</v>
@@ -4950,7 +4950,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B72">
         <v>2022</v>
@@ -4959,19 +4959,19 @@
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G72" s="8">
         <v>652905150122</v>
       </c>
       <c r="H72" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -4979,7 +4979,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B73">
         <v>2022</v>
@@ -4988,19 +4988,19 @@
         <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G73" s="8">
         <v>652905160121</v>
       </c>
       <c r="H73" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I73">
         <v>123</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B74">
         <v>2022</v>
@@ -5017,19 +5017,19 @@
         <v>12</v>
       </c>
       <c r="D74" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G74" s="8">
         <v>652905160213</v>
       </c>
       <c r="H74" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I74">
         <v>156</v>
@@ -5037,7 +5037,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B75">
         <v>2022</v>
@@ -5046,19 +5046,19 @@
         <v>12</v>
       </c>
       <c r="D75" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G75" s="8">
         <v>652905160220</v>
       </c>
       <c r="H75" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I75">
         <v>194</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B76">
         <v>2022</v>
@@ -5075,19 +5075,19 @@
         <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G76" s="8">
         <v>652905170120</v>
       </c>
       <c r="H76" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I76">
         <v>11</v>
@@ -5095,7 +5095,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B77">
         <v>2022</v>
@@ -5104,19 +5104,19 @@
         <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G77" s="8">
         <v>652905180129</v>
       </c>
       <c r="H77" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I77" s="4">
         <v>258</v>
@@ -5372,7 +5372,7 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.15">
@@ -5762,7 +5762,7 @@
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.15">
@@ -6002,7 +6002,7 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A172" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.15">
@@ -6027,7 +6027,7 @@
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A177" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.15">
@@ -6377,7 +6377,7 @@
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A247" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.15">
@@ -7147,7 +7147,7 @@
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A401" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update Physical Sales file to Exactly match Previous Royalty Run
Previous royalty run had two separate physical sales files. This update merged those numbers, so the results of the royalty run can more quickly be spot checked against the previous run.
</commit_message>
<xml_diff>
--- a/Physical_Sales.xlsx
+++ b/Physical_Sales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1780" windowWidth="28780" windowHeight="23920"/>
+    <workbookView xWindow="2160" yWindow="1780" windowWidth="30380" windowHeight="24360"/>
   </bookViews>
   <sheets>
     <sheet name="RS Physical Sales Template" sheetId="1" r:id="rId1"/>
@@ -2873,7 +2873,10 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2943,8 +2946,8 @@
       <c r="H2" t="s">
         <v>599</v>
       </c>
-      <c r="I2">
-        <v>112</v>
+      <c r="I2" s="8">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3089,7 +3092,7 @@
         <v>603</v>
       </c>
       <c r="I7">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -3147,7 +3150,7 @@
         <v>604</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3234,7 +3237,7 @@
         <v>607</v>
       </c>
       <c r="I12">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -3263,7 +3266,7 @@
         <v>607</v>
       </c>
       <c r="I13">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -3350,7 +3353,7 @@
         <v>610</v>
       </c>
       <c r="I16">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
@@ -3379,7 +3382,7 @@
         <v>611</v>
       </c>
       <c r="I17">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -3582,7 +3585,7 @@
         <v>618</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
@@ -3611,7 +3614,7 @@
         <v>619</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
@@ -3640,7 +3643,7 @@
         <v>620</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
@@ -3669,7 +3672,7 @@
         <v>621</v>
       </c>
       <c r="I27">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
@@ -3698,7 +3701,7 @@
         <v>622</v>
       </c>
       <c r="I28">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
@@ -3727,7 +3730,7 @@
         <v>623</v>
       </c>
       <c r="I29">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
@@ -4046,7 +4049,7 @@
         <v>634</v>
       </c>
       <c r="I40">
-        <v>73</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
@@ -4104,7 +4107,7 @@
         <v>636</v>
       </c>
       <c r="I42">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
@@ -4162,7 +4165,7 @@
         <v>638</v>
       </c>
       <c r="I44">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
@@ -4191,7 +4194,7 @@
         <v>639</v>
       </c>
       <c r="I45">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
@@ -4336,7 +4339,7 @@
         <v>643</v>
       </c>
       <c r="I50">
-        <v>53</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.15">
@@ -4394,7 +4397,7 @@
         <v>645</v>
       </c>
       <c r="I52">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.15">
@@ -4423,7 +4426,7 @@
         <v>646</v>
       </c>
       <c r="I53">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.15">
@@ -4452,7 +4455,7 @@
         <v>647</v>
       </c>
       <c r="I54">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.15">
@@ -4481,7 +4484,7 @@
         <v>648</v>
       </c>
       <c r="I55">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.15">
@@ -4510,7 +4513,7 @@
         <v>649</v>
       </c>
       <c r="I56">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.15">
@@ -4539,7 +4542,7 @@
         <v>650</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.15">
@@ -4568,7 +4571,7 @@
         <v>651</v>
       </c>
       <c r="I58">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
@@ -4626,7 +4629,7 @@
         <v>653</v>
       </c>
       <c r="I60">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.15">
@@ -4655,7 +4658,7 @@
         <v>654</v>
       </c>
       <c r="I61">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.15">
@@ -4684,7 +4687,7 @@
         <v>655</v>
       </c>
       <c r="I62">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.15">
@@ -4713,7 +4716,7 @@
         <v>656</v>
       </c>
       <c r="I63">
-        <v>435</v>
+        <v>455</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.15">
@@ -4742,7 +4745,7 @@
         <v>656</v>
       </c>
       <c r="I64">
-        <v>111</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
@@ -4800,7 +4803,7 @@
         <v>658</v>
       </c>
       <c r="I66">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.15">
@@ -4829,7 +4832,7 @@
         <v>658</v>
       </c>
       <c r="I67">
-        <v>62</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
@@ -4887,7 +4890,7 @@
         <v>660</v>
       </c>
       <c r="I69">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.15">
@@ -4916,7 +4919,7 @@
         <v>661</v>
       </c>
       <c r="I70">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.15">
@@ -4945,7 +4948,7 @@
         <v>662</v>
       </c>
       <c r="I71">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.15">
@@ -4974,7 +4977,7 @@
         <v>663</v>
       </c>
       <c r="I72">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.15">
@@ -5003,7 +5006,7 @@
         <v>664</v>
       </c>
       <c r="I73">
-        <v>123</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.15">
@@ -5032,7 +5035,7 @@
         <v>665</v>
       </c>
       <c r="I74">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
@@ -5061,7 +5064,7 @@
         <v>665</v>
       </c>
       <c r="I75">
-        <v>194</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
@@ -5090,7 +5093,7 @@
         <v>666</v>
       </c>
       <c r="I76">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.15">
@@ -5119,7 +5122,7 @@
         <v>667</v>
       </c>
       <c r="I77" s="4">
-        <v>258</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix label on Crazy Cool Christmas LP (correct from CD)
</commit_message>
<xml_diff>
--- a/Physical_Sales.xlsx
+++ b/Physical_Sales.xlsx
@@ -2873,10 +2873,10 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3222,7 +3222,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>495</v>

</xml_diff>